<commit_message>
Small fix to validate, documentation updates, testing files updates.
</commit_message>
<xml_diff>
--- a/tests/test_convert/testing_files/main_dir/mwtab_ms_conversion_directives_compare.xlsx
+++ b/tests/test_convert/testing_files/main_dir/mwtab_ms_conversion_directives_compare.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="124">
   <si>
     <t>#tags</t>
   </si>
@@ -379,13 +379,13 @@
     <t>matrix</t>
   </si>
   <si>
+    <t>#.values_to_str</t>
+  </si>
+  <si>
     <t>type=sample_prep</t>
   </si>
   <si>
     <t>type=treatment</t>
-  </si>
-  <si>
-    <t>#.values_to_str</t>
   </si>
 </sst>
 </file>
@@ -968,7 +968,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -979,7 +979,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -990,7 +990,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="B26" t="s">
         <v>19</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="B27" t="s">
         <v>20</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1177,8 +1177,11 @@
       <c r="I31" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -1202,6 +1205,9 @@
       </c>
       <c r="I32" t="s">
         <v>120</v>
+      </c>
+      <c r="J32" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1229,6 +1235,9 @@
       <c r="I33" t="s">
         <v>120</v>
       </c>
+      <c r="J33" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
@@ -1262,7 +1271,7 @@
         <v>94</v>
       </c>
       <c r="K35" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1568,7 +1577,7 @@
         <v>104</v>
       </c>
       <c r="J53" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K53" t="s">
         <v>95</v>
@@ -1600,7 +1609,7 @@
         <v>104</v>
       </c>
       <c r="J54" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K54" t="s">
         <v>95</v>
@@ -1632,7 +1641,7 @@
         <v>104</v>
       </c>
       <c r="J55" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K55" t="s">
         <v>95</v>
@@ -1986,7 +1995,7 @@
         <v>104</v>
       </c>
       <c r="J77" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K77" t="s">
         <v>95</v>
@@ -2018,7 +2027,7 @@
         <v>104</v>
       </c>
       <c r="J78" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K78" t="s">
         <v>95</v>
@@ -2050,7 +2059,7 @@
         <v>104</v>
       </c>
       <c r="J79" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K79" t="s">
         <v>95</v>

</xml_diff>